<commit_message>
Uploaded log for 15.9.2025. Uploaded Humerus of Wing10. It is separated into different portions for printing out of vero (polyjet) and nylon PA12. Still need to complete modifying the shoulder pulley of Humerus. Updated working hours.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F13B3B3-457D-448D-B978-A5AF25FB6C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772C9ED5-48FC-4299-A870-7E5C6130DEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>13.9.2025</t>
+  </si>
+  <si>
+    <t>15.9.2025</t>
   </si>
 </sst>
 </file>
@@ -364,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -477,6 +480,23 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded log for today. Finished designing Humerus, separated into two parts (ElbowPulley will be printed using vero (PolyJet) and Bone will be printed using nylon PA12 (SLS or MJF)). Finished designing ServoHolder with stiffened tube holding columns. Going to print and test the ServoHolder.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772C9ED5-48FC-4299-A870-7E5C6130DEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725C9F6A-83B4-4E1C-B617-C77E756F93D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>15.9.2025</t>
+  </si>
+  <si>
+    <t>16.9.2025</t>
   </si>
 </sst>
 </file>
@@ -367,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,6 +500,23 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.5625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded log for today. Started designing Radius. Created folder for receipts after 13.9.2025. Updated working hours.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725C9F6A-83B4-4E1C-B617-C77E756F93D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1ABCCC-B12E-46D8-9853-C6F6C576ED8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>16.9.2025</t>
+  </si>
+  <si>
+    <t>17.9.2025</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,6 +520,23 @@
         <v>0.5625</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.96527777777777779</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded log for today. Finished fixing the servo brackets. Finished designing Radius. Updated working hours.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1ABCCC-B12E-46D8-9853-C6F6C576ED8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC2A0F3-9107-439D-A1AD-F3763572FCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>17.9.2025</t>
+  </si>
+  <si>
+    <t>18.9.2025</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -537,6 +540,23 @@
         <v>0.96527777777777779</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.90972222222222221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded today's log. Finished designing ShoulderBracket and one Finger for printing using PA12. Redesigned ShoulderGear for efficient meshing. Updated working hours.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC2A0F3-9107-439D-A1AD-F3763572FCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19764319-B925-4318-9248-C08D1E7B7014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>18.9.2025</t>
+  </si>
+  <si>
+    <t>20.9.2025</t>
   </si>
 </sst>
 </file>
@@ -376,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,6 +560,23 @@
         <v>0.90972222222222221</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded log for today. Worked on installing modified servo brackets into the existing wing platform. Modified KST servo brackets for printing again. Finished improving the flap gears and modifying the Dynamixel servo holder accordingly. Updated working hours.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19764319-B925-4318-9248-C08D1E7B7014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26788664-F47C-4ED4-98B5-6295B7ED4AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>20.9.2025</t>
+  </si>
+  <si>
+    <t>23.9.2025</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,6 +580,23 @@
         <v>0.875</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded logs for yesterday and today. Started preparing to use in-context modelling for the whole design, which will ensure better linking between dimensions of the parts and better fit. Tested the elbow movement at 5 Hz. Updated working hours.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26788664-F47C-4ED4-98B5-6295B7ED4AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86D300-9BB7-474A-97CE-3588C92B3FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>23.9.2025</t>
+  </si>
+  <si>
+    <t>24.9.2025</t>
+  </si>
+  <si>
+    <t>25.9.2025</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,6 +603,28 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.78125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Today, I pushed all the progress made since last commit.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMF\BatWingProject\Drawings\Wing10\BatWing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86D300-9BB7-474A-97CE-3588C92B3FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC6083E-1045-4B9E-8750-426B6740F3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="170" windowWidth="25240" windowHeight="13510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,45 @@
   </si>
   <si>
     <t>25.9.2025</t>
+  </si>
+  <si>
+    <t>26.9.2025</t>
+  </si>
+  <si>
+    <t>27.9.2025</t>
+  </si>
+  <si>
+    <t>29.9.2025</t>
+  </si>
+  <si>
+    <t>1.10.2025</t>
+  </si>
+  <si>
+    <t>2.10.2025</t>
+  </si>
+  <si>
+    <t>6.10.2025</t>
+  </si>
+  <si>
+    <t>8.10.2025</t>
+  </si>
+  <si>
+    <t>10.10.2025</t>
+  </si>
+  <si>
+    <t>11.10.2025</t>
+  </si>
+  <si>
+    <t>13.10.2025</t>
+  </si>
+  <si>
+    <t>15.10.2025</t>
+  </si>
+  <si>
+    <t>16.10.2025</t>
+  </si>
+  <si>
+    <t>17.10.2025</t>
   </si>
 </sst>
 </file>
@@ -388,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,6 +664,191 @@
         <v>0.78125</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.50694444444444442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.5625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>